<commit_message>
feature: architecture and other optimizations
</commit_message>
<xml_diff>
--- a/autorun/ModelsLearning.xlsx
+++ b/autorun/ModelsLearning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/PycharmProjects/Yandex-specialization-ML/autorun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\PycharmProjects\Yandex-specialization-ML\autorun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57C092-66C7-514C-9298-D013B8295506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AA7582-2EC6-4233-B3C4-B56248B80A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="2260" windowWidth="28240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Version name</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>trainable</t>
+  </si>
+  <si>
+    <t>thirdModel</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>secondModel</t>
+  </si>
+  <si>
+    <t>Third</t>
   </si>
 </sst>
 </file>
@@ -396,20 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -434,6 +446,34 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
train first and second models
</commit_message>
<xml_diff>
--- a/autorun/ModelsLearning.xlsx
+++ b/autorun/ModelsLearning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\PycharmProjects\Yandex-specialization-ML\autorun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/PycharmProjects/Yandex-specialization-ML/autorun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A970D3A-24CC-4BA4-B7D3-117A3D04FD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A8E9D8-7036-2F4A-A940-1193AFF004A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Version name</t>
   </si>
@@ -43,19 +43,22 @@
     <t>firstModel</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>secondModel</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>thirdModel</t>
+  </si>
+  <si>
     <t>trainable</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>secondModel</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>thirdModel</t>
   </si>
 </sst>
 </file>
@@ -419,17 +422,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -458,7 +461,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -472,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -483,7 +486,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>